<commit_message>
week 7. Updated bf table
</commit_message>
<xml_diff>
--- a/2022S2/tutorial notes/completed example belmanford.xlsx
+++ b/2022S2/tutorial notes/completed example belmanford.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/edmundc1_student_unimelb_edu_au/Documents/COMP90054/2022S2/tutorial notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{8820C2D4-07A2-47DF-B2F5-9A332385199F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1348FB4D-BE67-45F3-B751-32979E94B0BD}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{8820C2D4-07A2-47DF-B2F5-9A332385199F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDEA51C1-09A1-4157-9BE2-6669358587AF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A494107E-2032-4C7B-AEA5-D7DFC63686CC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="25">
   <si>
     <t>i</t>
   </si>
@@ -126,14 +126,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,11 +163,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -494,7 +486,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,28 +495,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -545,43 +537,43 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" t="s">
         <v>15</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" t="s">
         <v>21</v>
       </c>
       <c r="T2" s="1" t="s">
@@ -654,10 +646,137 @@
       <c r="A4">
         <v>1</v>
       </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>1+E3+B3+K3</f>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>1+B3+E3+K3</f>
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f>1+E3+C3</f>
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D7" si="0">1+E4+B4+K4</f>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F7" si="1">1+B4+E4+K4</f>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G7" si="2">1+E4+C4</f>
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f>1+E4+D4+T4</f>
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <f>1+F4+B4</f>
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f>1+F4+C4</f>
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f>1+G4+B4</f>
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <f>1+G4+C4</f>
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <f>1+G4+D4</f>
+        <v>3</v>
+      </c>
+      <c r="O5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <f>1+F4</f>
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
@@ -665,17 +784,151 @@
         <f>A5+1</f>
         <v>3</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="T6" s="2"/>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H7" si="3">1+E5+D5+T5</f>
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I7" si="4">1+F5+B5</f>
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J7" si="5">1+F5+C5</f>
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ref="L6:L7" si="6">1+G5+B5</f>
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6:M7" si="7">1+G5+C5</f>
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6:N7" si="8">1+G5+D5</f>
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <f>1+H5+B5</f>
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <f>1+H5+C5</f>
+        <v>3</v>
+      </c>
+      <c r="Q6">
+        <f>1+H5+D5</f>
+        <v>4</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6:R7" si="9">1+F5</f>
+        <v>2</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="T7" s="1"/>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <f>1+H6+B6</f>
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <f>1+H6+C6</f>
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <f>1+H6+D6</f>
+        <v>4</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -683,32 +936,32 @@
       </c>
       <c r="B8">
         <f>SUM(J6,N6,T6)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -729,43 +982,43 @@
       <c r="F13" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" t="s">
         <v>11</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" t="s">
         <v>13</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" t="s">
         <v>14</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" t="s">
         <v>15</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="O13" t="s">
         <v>17</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="P13" t="s">
         <v>18</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="Q13" t="s">
         <v>19</v>
       </c>
-      <c r="R13" s="2" t="s">
+      <c r="R13" t="s">
         <v>20</v>
       </c>
-      <c r="S13" s="2" t="s">
+      <c r="S13" t="s">
         <v>21</v>
       </c>
       <c r="T13" s="1" t="s">
@@ -838,10 +1091,137 @@
       <c r="A15">
         <v>1</v>
       </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f>1+MAX(E14,B14,K14)</f>
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f>1+MAX(B14,E14,K14)</f>
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f>1+MAX(C14,E14,S14)</f>
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" t="s">
+        <v>1</v>
+      </c>
+      <c r="O15" t="s">
+        <v>1</v>
+      </c>
+      <c r="P15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:D18" si="10">1+MAX(E15,B15,K15)</f>
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16:F18" si="11">1+MAX(B15,E15,K15)</f>
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:G18" si="12">1+MAX(C15,E15,S15)</f>
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <f>1+MAX(E15,D15)</f>
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <f>1+MAX(F15,B15)</f>
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <f>1+MAX(F15,C15)</f>
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f>1+MAX(G15,B15)</f>
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <f>1+MAX(G15,C15)</f>
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <f>1+MAX(G15,D15)</f>
+        <v>2</v>
+      </c>
+      <c r="O16" t="s">
+        <v>1</v>
+      </c>
+      <c r="P16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <f>1+MAX(F15)</f>
+        <v>2</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
@@ -849,17 +1229,151 @@
         <f>A16+1</f>
         <v>3</v>
       </c>
-      <c r="J17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="T17" s="2"/>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ref="H17:H18" si="13">1+MAX(E16,D16)</f>
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17:I18" si="14">1+MAX(F16,B16)</f>
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ref="J17:J18" si="15">1+MAX(F16,C16)</f>
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ref="L17:L18" si="16">1+MAX(G16,B16)</f>
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ref="M17:M18" si="17">1+MAX(G16,C16)</f>
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <f t="shared" ref="N17:N18" si="18">1+MAX(G16,D16)</f>
+        <v>2</v>
+      </c>
+      <c r="O17">
+        <f>1+MAX(H16,B16)</f>
+        <v>3</v>
+      </c>
+      <c r="P17">
+        <f>1+MAX(H16,C16)</f>
+        <v>3</v>
+      </c>
+      <c r="Q17">
+        <f>1+MAX(H16,D16)</f>
+        <v>3</v>
+      </c>
+      <c r="R17">
+        <f t="shared" ref="R17:R18" si="19">1+MAX(F16)</f>
+        <v>2</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
-      <c r="J18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="T18" s="1"/>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <f>1+MAX(H17,B17)</f>
+        <v>3</v>
+      </c>
+      <c r="P18">
+        <f>1+MAX(H17,C17)</f>
+        <v>3</v>
+      </c>
+      <c r="Q18">
+        <f>1+MAX(H17,D17)</f>
+        <v>3</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -867,7 +1381,7 @@
       </c>
       <c r="B19">
         <f>MAX(J17,N17,T17)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>